<commit_message>
Heat map now works perfectly, but the color range is atrocious.
</commit_message>
<xml_diff>
--- a/Copy of Per10KData1.xlsx
+++ b/Copy of Per10KData1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Location</t>
   </si>
@@ -183,141 +183,6 @@
   </si>
   <si>
     <t>CapitaRatio</t>
-  </si>
-  <si>
-    <t>12/10K</t>
-  </si>
-  <si>
-    <t>11/10K</t>
-  </si>
-  <si>
-    <t>13.2/10K</t>
-  </si>
-  <si>
-    <t>11.5/10K</t>
-  </si>
-  <si>
-    <t>14.1/10K</t>
-  </si>
-  <si>
-    <t>13/10K</t>
-  </si>
-  <si>
-    <t>21.7/10K</t>
-  </si>
-  <si>
-    <t>16.1/10K</t>
-  </si>
-  <si>
-    <t>13.7/10K</t>
-  </si>
-  <si>
-    <t>11.7/10K</t>
-  </si>
-  <si>
-    <t>12.2/10K</t>
-  </si>
-  <si>
-    <t>8.1/10K</t>
-  </si>
-  <si>
-    <t>15/10K</t>
-  </si>
-  <si>
-    <t>12.5/10K</t>
-  </si>
-  <si>
-    <t>12.1/10K</t>
-  </si>
-  <si>
-    <t>13.4/10K</t>
-  </si>
-  <si>
-    <t>14.5/10K</t>
-  </si>
-  <si>
-    <t>15.6/10K</t>
-  </si>
-  <si>
-    <t>21/10K</t>
-  </si>
-  <si>
-    <t>27/10K</t>
-  </si>
-  <si>
-    <t>18.3/10K</t>
-  </si>
-  <si>
-    <t>10.6/10K</t>
-  </si>
-  <si>
-    <t>16.4/10K</t>
-  </si>
-  <si>
-    <t>10.9/10K</t>
-  </si>
-  <si>
-    <t>10.1/10K</t>
-  </si>
-  <si>
-    <t>15.9/10K</t>
-  </si>
-  <si>
-    <t>16/10K</t>
-  </si>
-  <si>
-    <t>12.3/10K</t>
-  </si>
-  <si>
-    <t>22.5/10K</t>
-  </si>
-  <si>
-    <t>13.9/10K</t>
-  </si>
-  <si>
-    <t>17.9/10K</t>
-  </si>
-  <si>
-    <t>11.2/10K</t>
-  </si>
-  <si>
-    <t>14.4/10K</t>
-  </si>
-  <si>
-    <t>18.8/10K</t>
-  </si>
-  <si>
-    <t>22.23/10K</t>
-  </si>
-  <si>
-    <t>10.5/10K</t>
-  </si>
-  <si>
-    <t>14.75/10K</t>
-  </si>
-  <si>
-    <t>11.6/10K</t>
-  </si>
-  <si>
-    <t>17.4/10K</t>
-  </si>
-  <si>
-    <t>13.1/10K</t>
-  </si>
-  <si>
-    <t>14.7/10K</t>
-  </si>
-  <si>
-    <t>13.5/10K</t>
-  </si>
-  <si>
-    <t>14.6/10K</t>
-  </si>
-  <si>
-    <t>9.1/10K</t>
-  </si>
-  <si>
-    <t>56.9/10K</t>
   </si>
 </sst>
 </file>
@@ -700,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -722,408 +587,408 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>53</v>
+      <c r="B2" s="5">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>54</v>
+      <c r="B3" s="5">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>55</v>
+      <c r="B4" s="5">
+        <v>13.2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>56</v>
+      <c r="B5" s="5">
+        <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>57</v>
+      <c r="B6">
+        <v>14.1</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>58</v>
+      <c r="B7" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>59</v>
+      <c r="B8" s="6">
+        <v>21.7</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>60</v>
+      <c r="B9" s="6">
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>97</v>
+      <c r="B10" s="6">
+        <v>56.9</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>61</v>
+      <c r="B11">
+        <v>13.7</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>62</v>
+      <c r="B12">
+        <v>11.7</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>63</v>
+      <c r="B13" s="6">
+        <v>12.2</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>64</v>
+      <c r="B14" s="6">
+        <v>8.1</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>65</v>
+      <c r="B15">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>66</v>
+      <c r="B16" s="5">
+        <v>12.5</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>63</v>
+      <c r="B17" s="6">
+        <v>12.2</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>67</v>
+      <c r="B18" s="6">
+        <v>12.1</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>68</v>
+      <c r="B19" s="6">
+        <v>13.4</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>69</v>
+      <c r="B20" s="6">
+        <v>14.5</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>70</v>
+      <c r="B21" s="6">
+        <v>15.6</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>71</v>
+      <c r="B22" s="6">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>72</v>
+      <c r="B23" s="6">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>73</v>
+      <c r="B24" s="5">
+        <v>18.3</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>60</v>
+      <c r="B25" s="6">
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>74</v>
+      <c r="B26" s="6">
+        <v>10.6</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>75</v>
+      <c r="B27" s="6">
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>76</v>
+      <c r="B28" s="6">
+        <v>10.9</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>61</v>
+      <c r="B29" s="6">
+        <v>13.7</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>77</v>
+      <c r="B30" s="6">
+        <v>10.1</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>78</v>
+      <c r="B31" s="6">
+        <v>15.9</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>79</v>
+      <c r="B32" s="6">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>80</v>
+      <c r="B33" s="6">
+        <v>12.3</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>81</v>
+      <c r="B34">
+        <v>22.5</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>82</v>
+      <c r="B35" s="6">
+        <v>13.9</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>56</v>
+      <c r="B36" s="6">
+        <v>11.5</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>83</v>
+      <c r="B37">
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>84</v>
+      <c r="B38" s="6">
+        <v>11.2</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>85</v>
+      <c r="B39" s="6">
+        <v>14.4</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>86</v>
+      <c r="B40">
+        <v>18.8</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>87</v>
+      <c r="B41" s="6">
+        <v>22.2</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>66</v>
+      <c r="B42" s="6">
+        <v>12.5</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>88</v>
+      <c r="B43" s="6">
+        <v>10.5</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>89</v>
+      <c r="B44" s="6">
+        <v>14.8</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>62</v>
+      <c r="B45">
+        <v>11.7</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>90</v>
+      <c r="B46" s="6">
+        <v>11.6</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>91</v>
+      <c r="B47" s="6">
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>92</v>
+      <c r="B48" s="6">
+        <v>13.1</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>93</v>
+      <c r="B49" s="6">
+        <v>14.7</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>94</v>
+      <c r="B50" s="6">
+        <v>13.5</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>95</v>
+      <c r="B51" s="6">
+        <v>14.6</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>96</v>
+      <c r="B52" s="6">
+        <v>9.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>